<commit_message>
huzzah! successful proof of concept!
</commit_message>
<xml_diff>
--- a/think tank/fundamentals/v1.1/company-overview-demo.xlsx
+++ b/think tank/fundamentals/v1.1/company-overview-demo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,12 +443,552 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>Symbol</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Thank you for using Alpha Vantage! Our standard API call frequency is 5 calls per minute and 500 calls per day. Please visit https://www.alphavantage.co/premium/ if you would like to target a higher API call frequency.</t>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>AssetType</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Common Stock</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Agilent Technologies Inc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Agilent Technologies, Inc. is an American analytical instrumentation development and manufacturing company that offers its products and services to markets worldwide. Its global headquarters is located in Santa Clara, California.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CIK</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1090872</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Exchange</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LIFE SCIENCES</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>INSTRUMENTS FOR MEAS &amp; TESTING OF ELECTRICITY &amp; ELEC SIGNALS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5301 STEVENS CREEK BLVD, SANTA CLARA, CA, US</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>FiscalYearEnd</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>LatestQuarter</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2022-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MarketCapitalization</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>36208771000</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1922000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>PERatio</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>27.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>PEGRatio</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2.046</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>BookValue</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>DividendPerShare</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.824</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>DividendYield</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0.0069</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>EPS</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>4.38</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>RevenuePerShareTTM</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>22.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ProfitMargin</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.199</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>OperatingMarginTTM</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.239</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>ReturnOnAssetsTTM</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.095</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>ReturnOnEquityTTM</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>RevenueTTM</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>6659000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>GrossProfitTTM</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>3407000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>DilutedEPSTTM</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>4.38</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>QuarterlyEarningsGrowthYOY</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>QuarterlyRevenueGrowthYOY</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>0.083</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>AnalystTargetPrice</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>150.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>TrailingPE</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>27.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>ForwardPE</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>22.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>PriceToSalesRatioTTM</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>5.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>PriceToBookRatio</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>7.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>EVToRevenue</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>5.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>EVToEBITDA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>20.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Beta</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1.067</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>52WeekHigh</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>164.91</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>52WeekLow</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>112.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>50DayMovingAverage</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>130.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>200DayMovingAverage</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>131.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>SharesOutstanding</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>296041000</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>DividendDate</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2022-10-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>ExDividendDate</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2022-10-03</t>
         </is>
       </c>
     </row>

</xml_diff>